<commit_message>
fix input and output conventions
</commit_message>
<xml_diff>
--- a/SocialMediaAnalysis/inputData (Backup).xlsx
+++ b/SocialMediaAnalysis/inputData (Backup).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjak923\Documents\social-media-analysis\SocialMediaAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/xzha897_uoa_auckland_ac_nz/Documents/Documents/GitHub/social-media-analysis/SocialMediaAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8349CB7-9F47-4A4E-BEEF-F1265ACB3467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{E8349CB7-9F47-4A4E-BEEF-F1265ACB3467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF2890D2-DAE9-40B1-9E57-3530B8B87A23}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
-  <si>
-    <t xml:space="preserve">Topic </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Comment</t>
   </si>
   <si>
     <t>Result</t>
-  </si>
-  <si>
-    <t>Verizon</t>
   </si>
   <si>
     <t>thanks to michelle et al at @verizonsupport who helped push my no-show-phone problem along. order canceled successfully and ordered this for pickup today at the apple store in the mall</t>
@@ -322,92 +316,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="46.140625" customWidth="1"/>
-    <col min="3" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="46.140625" customWidth="1"/>
+    <col min="2" max="25" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
+      <c r="D2">
+        <v>0.73</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3">
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
         <v>0.92</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5">
+      <c r="D5">
         <v>0.56999999999999995</v>
       </c>
     </row>

</xml_diff>